<commit_message>
EPBDS-12620 Difference in error response structure between kafka and webservice call
</commit_message>
<xml_diff>
--- a/ITEST/itest.kafka.smoke/openl-repository/deployments/deployment1/simple1/Main.xlsx
+++ b/ITEST/itest.kafka.smoke/openl-repository/deployments/deployment1/simple1/Main.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\ITEST\itest.kafka.smoke\openl-repository\deployments\deployment1\simple1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E62FEDE-0093-4231-8FAD-987652A3725B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="13010" yWindow="6800" windowWidth="19210" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -14,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stanislav Shor</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -242,9 +248,6 @@
     <t>R40</t>
   </si>
   <si>
-    <t>Good Night</t>
-  </si>
-  <si>
     <t>greeting</t>
   </si>
   <si>
@@ -258,12 +261,15 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
+  </si>
+  <si>
+    <t>= error("fail")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -593,19 +599,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -958,36 +967,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+    <row r="3" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
-    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -998,10 +1009,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1010,22 +1021,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -1053,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>15</v>
       </c>
@@ -1091,8 +1102,8 @@
       <c r="D11" s="25">
         <v>23</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>16</v>
+      <c r="E11" s="27" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>